<commit_message>
Grafici di Frequenza aggiunti
</commit_message>
<xml_diff>
--- a/Datasets/European-Country/15-64.xlsx
+++ b/Datasets/European-Country/15-64.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UTENTE\git\SAD_Project\Datasets\Age_Datasets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Magistrale\Statistica e Analisi dei Dati\SAD_Project\Datasets\European-Country\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8CA22B3C-EECF-4F22-B129-C9858962037D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{1E636646-7DBF-48BC-9AD9-E86D0FEDD7CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OECD.Stat export" sheetId="1" r:id="rId1"/>
@@ -117,9 +117,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="#,##0.000_ ;\-#,##0.000\ "/>
+    <numFmt numFmtId="164" formatCode="#,##0.000_ ;\-#,##0.000\ "/>
   </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
@@ -644,10 +644,10 @@
     <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="20" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="20" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="20" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1007,25 +1007,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BI27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="BJ2" sqref="BJ1:BJ1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+    <col min="1" max="1" width="27.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:61" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="e">
         <f ca="1">DotStatQuery(#REF!)</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="2" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1210,7 +1210,7 @@
         <v>4.976</v>
       </c>
     </row>
-    <row r="3" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>4.6379999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>2.2970000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
@@ -1765,7 +1765,7 @@
         <v>2.9279999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1950,7 +1950,7 @@
         <v>5.1479999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -2135,7 +2135,7 @@
         <v>3.669</v>
       </c>
     </row>
-    <row r="8" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -2320,7 +2320,7 @@
         <v>4.4740000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -2505,7 +2505,7 @@
         <v>4.3529999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>7</v>
       </c>
@@ -2690,7 +2690,7 @@
         <v>4.7489999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>3.0649999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -3060,7 +3060,7 @@
         <v>3.3860000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
@@ -3245,7 +3245,7 @@
         <v>7.3609999999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
@@ -3430,7 +3430,7 @@
         <v>3.9129999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
@@ -3615,7 +3615,7 @@
         <v>3.125</v>
       </c>
     </row>
-    <row r="16" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -3800,7 +3800,7 @@
         <v>3.641</v>
       </c>
     </row>
-    <row r="17" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -3985,7 +3985,7 @@
         <v>9.0050000000000008</v>
       </c>
     </row>
-    <row r="18" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
@@ -4170,7 +4170,7 @@
         <v>4.4420000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
@@ -4355,7 +4355,7 @@
         <v>5.0819999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>16</v>
       </c>
@@ -4540,7 +4540,7 @@
         <v>3.359</v>
       </c>
     </row>
-    <row r="21" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>17</v>
       </c>
@@ -4725,7 +4725,7 @@
         <v>3.4590000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>2</v>
       </c>
@@ -4910,7 +4910,7 @@
         <v>3.8370000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>25</v>
       </c>
@@ -5095,7 +5095,7 @@
         <v>3.0379999999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>18</v>
       </c>
@@ -5280,7 +5280,7 @@
         <v>3.4239999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>19</v>
       </c>
@@ -5465,7 +5465,7 @@
         <v>3.6749999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>20</v>
       </c>
@@ -5650,7 +5650,7 @@
         <v>3.8620000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>21</v>
       </c>
@@ -5840,7 +5840,7 @@
     <sortCondition ref="A2:A27"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="A10" r:id="rId1" display="http://stats.oecd.org/OECDStat_Metadata/ShowMetadata.ashx?Dataset=EXP_MORSC&amp;Coords=[COU].[DEU]&amp;ShowOnWeb=true&amp;Lang=en"/>
+    <hyperlink ref="A10" r:id="rId1" display="http://stats.oecd.org/OECDStat_Metadata/ShowMetadata.ashx?Dataset=EXP_MORSC&amp;Coords=[COU].[DEU]&amp;ShowOnWeb=true&amp;Lang=en" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>